<commit_message>
eu-dga: fix SIP -> SIPProvider
</commit_message>
<xml_diff>
--- a/code/vocab_csv/eu-dga.xlsx
+++ b/code/vocab_csv/eu-dga.xlsx
@@ -272,7 +272,7 @@
     <t>SingleInformationPoint</t>
   </si>
   <si>
-    <t>Single Information Point</t>
+    <t>Single Information Point (SIP)</t>
   </si>
   <si>
     <t>Service responsible for receiving and transmiting requests for the re-use of public data</t>
@@ -728,7 +728,7 @@
     <t>An entity who is responsible for receiving and transmiting requests for the reuse of public data in the EU</t>
   </si>
   <si>
-    <t>eu-dga:SIP</t>
+    <t>eu-dga:SIPProvider</t>
   </si>
   <si>
     <t>DGA 8.4</t>
@@ -1147,6 +1147,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1154,9 +1157,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -5533,10 +5533,10 @@
       <c r="A2" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="38" t="s">
         <v>63</v>
       </c>
       <c r="D2" s="15" t="s">
@@ -5546,7 +5546,7 @@
         <v>65</v>
       </c>
       <c r="F2" s="10"/>
-      <c r="G2" s="38"/>
+      <c r="G2" s="39"/>
       <c r="H2" s="10"/>
       <c r="I2" s="25"/>
       <c r="J2" s="15"/>
@@ -5575,7 +5575,7 @@
       <c r="AE2" s="10"/>
     </row>
     <row r="3">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="39" t="s">
         <v>66</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -5591,10 +5591,10 @@
         <v>65</v>
       </c>
       <c r="F3" s="10"/>
-      <c r="G3" s="38"/>
+      <c r="G3" s="39"/>
       <c r="H3" s="10"/>
       <c r="I3" s="25"/>
-      <c r="J3" s="39" t="s">
+      <c r="J3" s="40" t="s">
         <v>69</v>
       </c>
       <c r="K3" s="13"/>
@@ -5628,17 +5628,17 @@
       <c r="B4" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="37" t="s">
         <v>73</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>65</v>
       </c>
       <c r="F4" s="10"/>
-      <c r="G4" s="38"/>
+      <c r="G4" s="39"/>
       <c r="H4" s="10"/>
       <c r="I4" s="25"/>
       <c r="J4" s="15"/>
@@ -5676,17 +5676,17 @@
       <c r="C5" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="37" t="s">
         <v>73</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>65</v>
       </c>
       <c r="F5" s="10"/>
-      <c r="G5" s="38"/>
+      <c r="G5" s="39"/>
       <c r="H5" s="10"/>
       <c r="I5" s="25"/>
-      <c r="J5" s="39" t="s">
+      <c r="J5" s="40" t="s">
         <v>77</v>
       </c>
       <c r="K5" s="13"/>
@@ -5720,20 +5720,20 @@
       <c r="B6" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="37" t="s">
         <v>73</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>65</v>
       </c>
       <c r="F6" s="10"/>
-      <c r="G6" s="38"/>
+      <c r="G6" s="39"/>
       <c r="H6" s="10"/>
       <c r="I6" s="25"/>
-      <c r="J6" s="39" t="s">
+      <c r="J6" s="40" t="s">
         <v>81</v>
       </c>
       <c r="K6" s="13"/>
@@ -5875,18 +5875,18 @@
       <c r="A2" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>83</v>
       </c>
       <c r="C2" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="38"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="44" t="s">
         <v>85</v>
       </c>
       <c r="F2" s="10"/>
-      <c r="G2" s="38"/>
+      <c r="G2" s="39"/>
       <c r="H2" s="10"/>
       <c r="I2" s="25"/>
       <c r="J2" s="15" t="s">
@@ -5926,12 +5926,12 @@
       <c r="C3" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="38"/>
+      <c r="D3" s="39"/>
       <c r="E3" s="44" t="s">
         <v>85</v>
       </c>
       <c r="F3" s="10"/>
-      <c r="G3" s="38"/>
+      <c r="G3" s="39"/>
       <c r="H3" s="10"/>
       <c r="I3" s="25"/>
       <c r="J3" s="15" t="s">
@@ -5962,21 +5962,21 @@
       <c r="AE3" s="10"/>
     </row>
     <row r="4">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="39" t="s">
         <v>92</v>
       </c>
       <c r="C4" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="44" t="s">
         <v>85</v>
       </c>
       <c r="F4" s="10"/>
-      <c r="G4" s="38"/>
+      <c r="G4" s="39"/>
       <c r="H4" s="10"/>
       <c r="I4" s="25"/>
       <c r="J4" s="15" t="s">
@@ -6010,18 +6010,18 @@
       <c r="A5" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="39" t="s">
         <v>95</v>
       </c>
       <c r="C5" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="39"/>
       <c r="E5" s="44" t="s">
         <v>85</v>
       </c>
       <c r="F5" s="10"/>
-      <c r="G5" s="38"/>
+      <c r="G5" s="39"/>
       <c r="H5" s="10"/>
       <c r="I5" s="25"/>
       <c r="J5" s="15" t="s">
@@ -6290,17 +6290,17 @@
       <c r="B3" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="39" t="s">
         <v>107</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>102</v>
       </c>
       <c r="F3" s="10"/>
-      <c r="G3" s="38"/>
+      <c r="G3" s="39"/>
       <c r="H3" s="10"/>
       <c r="I3" s="15" t="s">
         <v>108</v>
@@ -6331,10 +6331,10 @@
       <c r="AE3" s="10"/>
     </row>
     <row r="4">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="39" t="s">
         <v>110</v>
       </c>
       <c r="C4" s="43" t="s">
@@ -6378,10 +6378,10 @@
       <c r="AE4" s="10"/>
     </row>
     <row r="5">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="39" t="s">
         <v>114</v>
       </c>
       <c r="C5" s="43" t="s">
@@ -6565,17 +6565,17 @@
       <c r="B9" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="39" t="s">
         <v>120</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>102</v>
       </c>
       <c r="F9" s="10"/>
-      <c r="G9" s="38"/>
+      <c r="G9" s="39"/>
       <c r="H9" s="10"/>
       <c r="I9" s="49" t="s">
         <v>134</v>
@@ -6653,23 +6653,23 @@
       <c r="AE10" s="10"/>
     </row>
     <row r="11">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="D11" s="38"/>
+      <c r="D11" s="39"/>
       <c r="E11" s="11" t="s">
         <v>102</v>
       </c>
       <c r="F11" s="10"/>
-      <c r="G11" s="38"/>
+      <c r="G11" s="39"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="38" t="s">
+      <c r="I11" s="39" t="s">
         <v>143</v>
       </c>
       <c r="J11" s="25"/>
@@ -6745,10 +6745,10 @@
       <c r="AE12" s="10"/>
     </row>
     <row r="13">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="39" t="s">
         <v>150</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -6761,9 +6761,9 @@
         <v>129</v>
       </c>
       <c r="F13" s="10"/>
-      <c r="G13" s="38"/>
+      <c r="G13" s="39"/>
       <c r="H13" s="10"/>
-      <c r="I13" s="38" t="s">
+      <c r="I13" s="39" t="s">
         <v>153</v>
       </c>
       <c r="J13" s="25"/>
@@ -6839,25 +6839,25 @@
       <c r="AE14" s="10"/>
     </row>
     <row r="15">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="39" t="s">
         <v>160</v>
       </c>
       <c r="C15" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="39" t="s">
         <v>162</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>102</v>
       </c>
       <c r="F15" s="10"/>
-      <c r="G15" s="38"/>
+      <c r="G15" s="39"/>
       <c r="H15" s="10"/>
-      <c r="I15" s="38" t="s">
+      <c r="I15" s="39" t="s">
         <v>163</v>
       </c>
       <c r="J15" s="25"/>
@@ -6992,13 +6992,13 @@
       <c r="A2" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="39" t="s">
         <v>167</v>
       </c>
       <c r="E2" s="11" t="s">
@@ -7042,7 +7042,7 @@
       <c r="B3" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="38" t="s">
         <v>171</v>
       </c>
       <c r="D3" s="15" t="s">
@@ -7092,7 +7092,7 @@
       <c r="C4" s="43" t="s">
         <v>176</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="37" t="s">
         <v>177</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -7280,7 +7280,7 @@
       <c r="C8" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="37" t="s">
         <v>177</v>
       </c>
       <c r="E8" s="11" t="s">
@@ -7327,7 +7327,7 @@
       <c r="C9" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="37" t="s">
         <v>177</v>
       </c>
       <c r="E9" s="11" t="s">
@@ -7421,7 +7421,7 @@
       <c r="C11" s="43" t="s">
         <v>204</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="39" t="s">
         <v>205</v>
       </c>
       <c r="E11" s="11" t="s">
@@ -7459,7 +7459,7 @@
       <c r="AE11" s="10"/>
     </row>
     <row r="12">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="39" t="s">
         <v>207</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -7733,26 +7733,26 @@
       <c r="AE17" s="10"/>
     </row>
     <row r="18">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="39" t="s">
         <v>228</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="39" t="s">
         <v>229</v>
       </c>
       <c r="C18" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="39" t="s">
         <v>187</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>65</v>
       </c>
       <c r="F18" s="10"/>
-      <c r="G18" s="38"/>
+      <c r="G18" s="39"/>
       <c r="H18" s="10"/>
       <c r="I18" s="25"/>
-      <c r="J18" s="38" t="s">
+      <c r="J18" s="39" t="s">
         <v>231</v>
       </c>
       <c r="K18" s="10"/>
@@ -7876,17 +7876,17 @@
       <c r="B2" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="40" t="s">
+      <c r="D2" s="39"/>
+      <c r="E2" s="37" t="s">
         <v>238</v>
       </c>
       <c r="F2" s="52" t="s">
         <v>239</v>
       </c>
-      <c r="G2" s="38"/>
+      <c r="G2" s="39"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="53" t="s">
@@ -7922,11 +7922,11 @@
       <c r="B3" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="38" t="s">
         <v>243</v>
       </c>
       <c r="D3" s="43"/>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="37" t="s">
         <v>244</v>
       </c>
       <c r="F3" s="52" t="s">
@@ -7966,17 +7966,17 @@
       <c r="B4" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="38" t="s">
         <v>247</v>
       </c>
       <c r="D4" s="43"/>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="37" t="s">
         <v>248</v>
       </c>
       <c r="F4" s="52" t="s">
         <v>239</v>
       </c>
-      <c r="G4" s="38"/>
+      <c r="G4" s="39"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
@@ -8010,17 +8010,17 @@
       <c r="B5" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="38" t="s">
         <v>251</v>
       </c>
       <c r="D5" s="43"/>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="37" t="s">
         <v>252</v>
       </c>
       <c r="F5" s="52" t="s">
         <v>239</v>
       </c>
-      <c r="G5" s="38"/>
+      <c r="G5" s="39"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
@@ -8058,7 +8058,7 @@
         <v>255</v>
       </c>
       <c r="D6" s="10"/>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="37" t="s">
         <v>177</v>
       </c>
       <c r="F6" s="52" t="s">

</xml_diff>

<commit_message>
fix #346 incorrect space in EU-DGA
Co-authored-by: Arthit Suriyawongkul <arthit@gmail.com>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/eu-dga.xlsx
+++ b/code/vocab_csv/eu-dga.xlsx
@@ -562,7 +562,7 @@
     <t>Data Asset List</t>
   </si>
   <si>
-    <t>Searchable asset list which contains available data resources including their data format and size and the conditions for their re-use</t>
+    <t>Searchable asset list which contains available data resources including their data format and size and the conditions for their re-use</t>
   </si>
   <si>
     <t>DGA 8.2</t>
@@ -10593,7 +10593,7 @@
       <c r="B7" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="11" t="s">
         <v>158</v>
       </c>
       <c r="D7" s="10"/>

</xml_diff>